<commit_message>
Community Learning Report Template Tabs
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/CommunityLearningReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/CommunityLearningReportTemplate.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GIT\RS1920\src\ESFA.DC.ILR.ReportService.Reports\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Git\DC-ILR-1920-ReportService\src\ESFA.DC.ILR.ReportService.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D66B1B-6C2A-4AE4-8665-116A826EB177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0837A90-85A7-4EF2-A6A3-63AC315202B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28560" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Community Learning Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Community Learning Report'!$A$1:$I$42</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -517,29 +515,29 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -937,21 +935,21 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H22" sqref="H22:I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.3515625" customWidth="1"/>
-    <col min="2" max="2" width="14.87890625" customWidth="1"/>
-    <col min="3" max="3" width="14.234375" customWidth="1"/>
-    <col min="4" max="4" width="17.8203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5859375" customWidth="1"/>
-    <col min="6" max="6" width="3.5859375" customWidth="1"/>
-    <col min="7" max="7" width="9.41015625" customWidth="1"/>
-    <col min="8" max="8" width="12.5859375" customWidth="1"/>
-    <col min="9" max="9" width="8.41015625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.86328125" customWidth="1"/>
+    <col min="3" max="3" width="14.19921875" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" customWidth="1"/>
+    <col min="6" max="6" width="3.59765625" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" customWidth="1"/>
+    <col min="9" max="9" width="8.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -969,7 +967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -980,7 +978,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -995,7 +993,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1010,7 +1008,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1029,7 +1027,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1040,7 +1038,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
@@ -1053,7 +1051,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1064,318 +1062,318 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27" t="s">
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="27"/>
-    </row>
-    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="28" t="s">
+      <c r="I9" s="29"/>
+    </row>
+    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26" t="s">
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="26"/>
-    </row>
-    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="29" t="s">
+      <c r="I10" s="28"/>
+    </row>
+    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-    </row>
-    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="28" t="s">
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+    </row>
+    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26" t="s">
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="26"/>
-    </row>
-    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="28" t="s">
+      <c r="I12" s="28"/>
+    </row>
+    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26" t="s">
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="I13" s="28"/>
+    </row>
+    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-    </row>
-    <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="28" t="s">
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26" t="s">
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="26"/>
-    </row>
-    <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="I15" s="28"/>
+    </row>
+    <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-    </row>
-    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="28" t="s">
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+    </row>
+    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26" t="s">
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="I17" s="26"/>
-    </row>
-    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+      <c r="I17" s="28"/>
+    </row>
+    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-    </row>
-    <row r="19" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="31" t="s">
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+    </row>
+    <row r="19" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26" t="s">
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="26"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="29" t="s">
+      <c r="I19" s="28"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-    </row>
-    <row r="21" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="28" t="s">
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+    </row>
+    <row r="21" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26" t="s">
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="I21" s="26"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="28" t="s">
+      <c r="I21" s="28"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26" t="s">
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="I22" s="26"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="I22" s="28"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="28" t="s">
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26" t="s">
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="I24" s="26"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="29" t="s">
+      <c r="I24" s="28"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="28" t="s">
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26" t="s">
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="I26" s="26"/>
-    </row>
-    <row r="27" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="28" t="s">
+      <c r="I26" s="28"/>
+    </row>
+    <row r="27" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26" t="s">
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="26"/>
-    </row>
-    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="I27" s="28"/>
+    </row>
+    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -1386,7 +1384,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
         <v>27</v>
       </c>
@@ -1399,7 +1397,7 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
         <v>19</v>
       </c>
@@ -1412,7 +1410,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
         <v>20</v>
       </c>
@@ -1425,7 +1423,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="7" t="s">
         <v>28</v>
       </c>
@@ -1438,7 +1436,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="7" t="s">
         <v>23</v>
       </c>
@@ -1451,7 +1449,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="17" t="s">
         <v>29</v>
       </c>
@@ -1464,7 +1462,7 @@
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:9" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="17" t="s">
         <v>30</v>
       </c>
@@ -1477,7 +1475,7 @@
       <c r="H35" s="18"/>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1488,7 +1486,7 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1499,22 +1497,22 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E38" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-    </row>
-    <row r="39" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+    </row>
+    <row r="39" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="13" t="s">
         <v>16</v>
       </c>
@@ -1525,15 +1523,15 @@
       <c r="D39" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-    </row>
-    <row r="40" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+    </row>
+    <row r="40" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="13" t="s">
         <v>31</v>
       </c>
@@ -1544,30 +1542,30 @@
       <c r="D40" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-    </row>
-    <row r="41" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+    </row>
+    <row r="41" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-    </row>
-    <row r="42" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+    </row>
+    <row r="42" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="23" t="s">
         <v>41</v>
       </c>
@@ -1582,7 +1580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1595,6 +1593,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
@@ -1611,78 +1654,9 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H27:I27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
91286 - Update to CL Report template to make page start at correct cell A1
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/CommunityLearningReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/CommunityLearningReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Git\DC-ILR-1920-ReportService\src\ESFA.DC.ILR.ReportService.Reports\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley Beecham\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0837A90-85A7-4EF2-A6A3-63AC315202B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BCD7FF8-418A-4D4B-9E4C-84F8950CD630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Community Learning Report" sheetId="1" r:id="rId1"/>
@@ -515,29 +515,29 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -935,21 +935,19 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:I22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.86328125" customWidth="1"/>
-    <col min="3" max="3" width="14.19921875" customWidth="1"/>
-    <col min="4" max="4" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.59765625" customWidth="1"/>
-    <col min="6" max="6" width="3.59765625" customWidth="1"/>
-    <col min="7" max="7" width="9.3984375" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" customWidth="1"/>
-    <col min="9" max="9" width="8.3984375" customWidth="1"/>
+    <col min="1" max="1" width="17.3515625" customWidth="1"/>
+    <col min="2" max="2" width="14.87890625" customWidth="1"/>
+    <col min="3" max="3" width="14.17578125" customWidth="1"/>
+    <col min="4" max="4" width="17.8203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5859375" customWidth="1"/>
+    <col min="6" max="6" width="3.5859375" customWidth="1"/>
+    <col min="7" max="7" width="9.41015625" customWidth="1"/>
+    <col min="8" max="8" width="12.5859375" customWidth="1"/>
+    <col min="9" max="9" width="8.41015625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -967,7 +965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -978,7 +976,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -993,7 +991,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1008,7 +1006,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1027,7 +1025,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1038,7 +1036,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
@@ -1051,7 +1049,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1062,318 +1060,318 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29" t="s">
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="29"/>
-    </row>
-    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="24" t="s">
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28" t="s">
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="28"/>
-    </row>
-    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="26" t="s">
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-    </row>
-    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="24" t="s">
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+    </row>
+    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28" t="s">
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="28"/>
-    </row>
-    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="24" t="s">
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28" t="s">
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="28"/>
-    </row>
-    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+      <c r="I13" s="26"/>
+    </row>
+    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-    </row>
-    <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="24" t="s">
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28" t="s">
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="28"/>
-    </row>
-    <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-    </row>
-    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="24" t="s">
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+    </row>
+    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28" t="s">
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="I17" s="28"/>
-    </row>
-    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-    </row>
-    <row r="19" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="27" t="s">
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+    </row>
+    <row r="19" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28" t="s">
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="28"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="26" t="s">
+      <c r="I19" s="26"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-    </row>
-    <row r="21" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="24" t="s">
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28" t="s">
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="I21" s="28"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="24" t="s">
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
       <c r="D22" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28" t="s">
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="I22" s="28"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="24" t="s">
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28" t="s">
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="I24" s="28"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="26" t="s">
+      <c r="I24" s="26"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="24" t="s">
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28" t="s">
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="I26" s="28"/>
-    </row>
-    <row r="27" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="24" t="s">
+      <c r="I26" s="26"/>
+    </row>
+    <row r="27" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28" t="s">
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="28"/>
-    </row>
-    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I27" s="26"/>
+    </row>
+    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -1384,7 +1382,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A29" s="7" t="s">
         <v>27</v>
       </c>
@@ -1397,7 +1395,7 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" s="7" t="s">
         <v>19</v>
       </c>
@@ -1410,7 +1408,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A31" s="7" t="s">
         <v>20</v>
       </c>
@@ -1423,7 +1421,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A32" s="7" t="s">
         <v>28</v>
       </c>
@@ -1436,7 +1434,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A33" s="7" t="s">
         <v>23</v>
       </c>
@@ -1449,7 +1447,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A34" s="17" t="s">
         <v>29</v>
       </c>
@@ -1462,7 +1460,7 @@
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A35" s="17" t="s">
         <v>30</v>
       </c>
@@ -1475,7 +1473,7 @@
       <c r="H35" s="18"/>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1486,7 +1484,7 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1497,22 +1495,22 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-    </row>
-    <row r="39" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+    </row>
+    <row r="39" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A39" s="13" t="s">
         <v>16</v>
       </c>
@@ -1523,15 +1521,15 @@
       <c r="D39" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="30" t="s">
+      <c r="E39" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-    </row>
-    <row r="40" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+    </row>
+    <row r="40" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="13" t="s">
         <v>31</v>
       </c>
@@ -1542,30 +1540,30 @@
       <c r="D40" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="30" t="s">
+      <c r="E40" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-    </row>
-    <row r="41" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+    </row>
+    <row r="41" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="E41" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
-    </row>
-    <row r="42" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+    </row>
+    <row r="42" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A42" s="23" t="s">
         <v>41</v>
       </c>
@@ -1580,7 +1578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1593,6 +1591,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="E41:I41"/>
     <mergeCell ref="E40:I40"/>
     <mergeCell ref="E39:I39"/>
@@ -1609,51 +1652,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Community Learning Report 2021 Rollover
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/CommunityLearningReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/CommunityLearningReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley Beecham\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GIT\RS2021\src\ESFA.DC.ILR.ReportService.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BCD7FF8-418A-4D4B-9E4C-84F8950CD630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D96FBE7-1AC3-4099-A909-65B9B307DCBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t>Summary of Learners by Non-Single-Budget Category</t>
   </si>
@@ -170,9 +170,6 @@
     <t xml:space="preserve">    in this report</t>
   </si>
   <si>
-    <t>Application Version</t>
-  </si>
-  <si>
     <t>&amp;=CommunityLearning.ProviderName</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
   </si>
   <si>
     <t>&amp;=CommunityLearning.FilePreparationDate</t>
-  </si>
-  <si>
-    <t>&amp;=CommunityLearning.ApplicationVersion</t>
   </si>
   <si>
     <t>&amp;=CommunityLearning.TotalCommunityLearning.TotalLearners</t>
@@ -515,29 +509,29 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -981,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="5"/>
@@ -996,7 +990,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="5"/>
@@ -1011,7 +1005,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="5"/>
@@ -1019,10 +1013,10 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
@@ -1061,315 +1055,315 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27" t="s">
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="27"/>
+      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="I10" s="28"/>
+    </row>
+    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+    </row>
+    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26" t="s">
+      <c r="E12" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="26"/>
-    </row>
-    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="29" t="s">
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="28"/>
+    </row>
+    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="28"/>
+    </row>
+    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="28"/>
+    </row>
+    <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+    </row>
+    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="28"/>
+    </row>
+    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+    </row>
+    <row r="19" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="28"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-    </row>
-    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="28" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+    </row>
+    <row r="21" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="26"/>
-    </row>
-    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="28" t="s">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="28"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-    </row>
-    <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="26"/>
-    </row>
-    <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-    </row>
-    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="I17" s="26"/>
-    </row>
-    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-    </row>
-    <row r="19" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="I19" s="26"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="29" t="s">
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="28"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="28"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-    </row>
-    <row r="21" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="28" t="s">
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" s="26"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="28" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" s="28"/>
+    </row>
+    <row r="27" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="26"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="I24" s="26"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="26" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26" t="s">
+      <c r="E27" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="I26" s="26"/>
-    </row>
-    <row r="27" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="20" t="s">
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I27" s="26"/>
+      <c r="I27" s="28"/>
     </row>
     <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" s="9"/>
@@ -1502,51 +1496,47 @@
       <c r="D38" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
+      <c r="E38" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
     </row>
     <row r="39" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A39" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" s="14"/>
       <c r="D39" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
+      <c r="E39" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
     </row>
     <row r="40" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>43</v>
-      </c>
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
+      <c r="E40" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
     </row>
     <row r="41" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A41" s="5"/>
@@ -1555,17 +1545,17 @@
       <c r="D41" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
+      <c r="E41" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
     </row>
     <row r="42" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A42" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -1591,6 +1581,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
@@ -1607,51 +1642,6 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H27:I27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>